<commit_message>
moved into folder, added introduction
</commit_message>
<xml_diff>
--- a/ComparisionSummary.xlsx
+++ b/ComparisionSummary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\NCProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cools\Desktop\GitHub\NCProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E7C80E-7B25-4E6B-88DE-70D721B9D811}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6231EB4E-576C-48C1-AB67-6D1843D34048}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="1470" windowWidth="14700" windowHeight="11385" xr2:uid="{1C1BFC6E-BC39-4437-BC91-90D09A30A678}"/>
+    <workbookView xWindow="8355" yWindow="1635" windowWidth="14670" windowHeight="11385" xr2:uid="{1C1BFC6E-BC39-4437-BC91-90D09A30A678}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>Super Linear</t>
   </si>
   <si>
-    <t>Methode Approach</t>
-  </si>
-  <si>
     <t>MidPoint</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>Prog Effect</t>
+  </si>
+  <si>
+    <t>Method of Approach</t>
   </si>
 </sst>
 </file>
@@ -152,13 +152,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="justify"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,10 +483,13 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="14.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
@@ -499,7 +508,7 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -516,111 +525,111 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>2</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>1</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>2</v>
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>23</v>
+      <c r="E8" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F8" s="2"/>
     </row>

</xml_diff>